<commit_message>
Added XL Sheet to MongoDB
</commit_message>
<xml_diff>
--- a/backend/student_template.xlsx
+++ b/backend/student_template.xlsx
@@ -1,57 +1,43 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
-  <workbookPr defaultThemeVersion="124226"/>
-  <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
-  </bookViews>
+  <workbookPr codeName="ThisWorkbook"/>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
-  <si>
-    <t>studentName</t>
-  </si>
-  <si>
-    <t>studentEmail</t>
-  </si>
-  <si>
-    <t>studentPhone</t>
-  </si>
-  <si>
-    <t>studentCourseName</t>
-  </si>
-  <si>
-    <t>studentCourseCompleted</t>
-  </si>
-  <si>
-    <t>certificateId</t>
-  </si>
-  <si>
-    <t>expireDate</t>
-  </si>
-</sst>
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:vt="http://schemas.openxmlformats.org/officeDocument/2006/docPropsVTypes">
+  <numFmts count="1">
+    <numFmt numFmtId="56" formatCode="&quot;上午/下午 &quot;hh&quot;時&quot;mm&quot;分&quot;ss&quot;秒 &quot;"/>
+  </numFmts>
+  <fonts count="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -66,7 +52,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -74,36 +60,18 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
+  <cellXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
 </styleSheet>
 </file>
 
@@ -182,6 +150,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -216,6 +185,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -250,20 +220,16 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:shade val="51000"/>
+                <a:tint val="100000"/>
+                <a:shade val="100000"/>
                 <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="80000">
-              <a:schemeClr val="phClr">
-                <a:shade val="93000"/>
-                <a:satMod val="130000"/>
-              </a:schemeClr>
-            </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="94000"/>
-                <a:satMod val="135000"/>
+                <a:tint val="50000"/>
+                <a:shade val="100000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
@@ -385,43 +351,137 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
-  <a:objectDefaults/>
+  <a:objectDefaults>
+    <a:spDef>
+      <a:spPr/>
+      <a:bodyPr/>
+      <a:lstStyle/>
+      <a:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="3">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </a:style>
+    </a:spDef>
+    <a:lnDef>
+      <a:spPr/>
+      <a:bodyPr/>
+      <a:lstStyle/>
+      <a:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </a:style>
+    </a:lnDef>
+  </a:objectDefaults>
   <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:7">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
+    <row r="1">
+      <c r="A1" t="str">
+        <v>studentName</v>
+      </c>
+      <c r="B1" t="str">
+        <v>studentEmail</v>
+      </c>
+      <c r="C1" t="str">
+        <v>studentPhone</v>
+      </c>
+      <c r="D1" t="str">
+        <v>studentCourseName</v>
+      </c>
+      <c r="E1" t="str">
+        <v>studentCourseCompleted</v>
+      </c>
+      <c r="F1" t="str">
+        <v>certificateId</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="str">
+        <v>Venkatesh</v>
+      </c>
+      <c r="B2" t="str">
+        <v>ven@gmail.com</v>
+      </c>
+      <c r="C2">
+        <v>9998887776</v>
+      </c>
+      <c r="D2" t="str">
+        <v>Full Stack Web Development</v>
+      </c>
+      <c r="E2" t="b">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
+      <c r="F2" t="str">
+        <v>BLFSWB4296</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="str">
+        <v>Nadeem</v>
+      </c>
+      <c r="B3" t="str">
+        <v>nadeem@gmail.com</v>
+      </c>
+      <c r="C3">
+        <v>9888777666</v>
+      </c>
+      <c r="D3" t="str">
+        <v>AWS</v>
+      </c>
+      <c r="E3" t="str">
+        <v>TRUE</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>Priya</v>
+      </c>
+      <c r="B4" t="str">
+        <v>priya@gmail.com</v>
+      </c>
+      <c r="C4" t="str">
+        <v>9900088877</v>
+      </c>
+      <c r="D4" t="str">
+        <v>Gen AI</v>
+      </c>
+      <c r="E4" t="b">
+        <v>1</v>
+      </c>
+      <c r="F4" t="str">
+        <v>BLGAI9637</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <ignoredErrors>
+    <ignoredError numberStoredAsText="1" sqref="A1:F4"/>
+  </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>